<commit_message>
Desenvolvendo análise de correlação entre salario minimo e valor dos carros
</commit_message>
<xml_diff>
--- a/Salario Minimo.xlsx
+++ b/Salario Minimo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nishbdorg-my.sharepoint.com/personal/154_365net_co/Documents/Projetos/TabelaFiPY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F95C554-35F6-4E42-946E-1D1E6F346B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8F95C554-35F6-4E42-946E-1D1E6F346B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3208642C-8131-4EB0-9B47-F86180B65ED2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B64E535-8FFF-4858-99C5-37D3A3506264}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Salário mínimo vigente</t>
+    <t>Salario</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C049FE4-77C8-4D00-9062-81595C2632DB}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection sqref="A1:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>